<commit_message>
fix test data (remove underscores)
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_autoid.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_autoid.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="1580" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="6" r:id="rId1"/>
@@ -557,13 +557,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>